<commit_message>
- code refactoring - added new feature for debugging the tests more easily
</commit_message>
<xml_diff>
--- a/examples-simple/src/test/resources/ArithmeticalTests2.xlsx
+++ b/examples-simple/src/test/resources/ArithmeticalTests2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="First arithmetical Test" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
   <si>
     <t>disabled</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>With a second parameter, but only one header column.</t>
+  </si>
+  <si>
+    <t>breakpoint</t>
   </si>
 </sst>
 </file>
@@ -452,18 +455,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -471,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -485,7 +488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -499,7 +502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -513,7 +516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -524,7 +527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -538,7 +541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -552,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -565,8 +568,11 @@
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -578,6 +584,9 @@
       </c>
       <c r="D15">
         <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -651,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bugfix: disable single test-commands
</commit_message>
<xml_diff>
--- a/examples-simple/src/test/resources/ArithmeticalTests2.xlsx
+++ b/examples-simple/src/test/resources/ArithmeticalTests2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\jexunit\examples-simple\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="26">
   <si>
     <t>disabled</t>
   </si>
@@ -162,14 +167,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -207,9 +215,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,7 +252,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,7 +287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -453,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,23 +639,57 @@
         <v>6</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21">
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E24" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>